<commit_message>
add scale in worksheet xml
</commit_message>
<xml_diff>
--- a/tests/data/11_print_settings.xlsx
+++ b/tests/data/11_print_settings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/"/>
     </mc:Choice>
@@ -419,7 +419,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" scale="100"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;14&amp;K000000left header&amp;C&amp;"Calibri,Regular"&amp;KFB0006center header&amp;R&amp;"Comic Sans MS Bold,Bold"&amp;U&amp;K000000right header</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000left &amp;&amp; footer&amp;Ccenter footer&amp;Rright footer</oddFooter>

</xml_diff>